<commit_message>
[fix&add] conflict, remove file
</commit_message>
<xml_diff>
--- a/experiment/result/result_ex2.xlsx
+++ b/experiment/result/result_ex2.xlsx
@@ -1,20 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smari\Documents\assist-create-package-design\experiment\result\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0193A4B9-CFB2-4AB3-939E-AE623B027DF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C138A6-B7E6-4A49-9290-7113629A59DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" xr2:uid="{03C62BA8-FA6A-4E93-8153-8531E82091E0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11620" activeTab="1" xr2:uid="{03C62BA8-FA6A-4E93-8153-8531E82091E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet2!$A$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet2!$A$3</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Sheet2!$A$3</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Sheet2!$A$4</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Sheet2!$A$5</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Sheet2!$B$1:$G$1</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Sheet2!$B$2:$G$2</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Sheet2!$B$3:$G$3</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">Sheet2!$B$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">Sheet2!$B$5:$G$5</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$A$4</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$A$5</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$B$1:$G$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$B$2:$G$2</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet2!$B$3:$G$3</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet2!$B$4:$G$4</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet2!$B$5:$G$5</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet2!$A$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,13 +54,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>file size(h)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>index</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>30 2</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -96,6 +121,13 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFAB8B8"/>
+      <color rgb="FFF78D8D"/>
+      <color rgb="FFF75353"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -105,6 +137,1222 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ja-JP"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>600px: 最小値</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$2:$G$2</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>19536</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19293</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>11034</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4401</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-798C-490E-AE45-567B25F38FE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>600px: 平均値</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$3:$G$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>29892.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25995</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25633.5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15521.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8320.75</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4071</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-798C-490E-AE45-567B25F38FE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>30px: 最小値</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>23067</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22932</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12297</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5265</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4770</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-798C-490E-AE45-567B25F38FE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>30px: 平均値</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$1:$G$1</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>35037.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>28716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29175.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17604.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8615.25</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4770</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-798C-490E-AE45-567B25F38FE2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="509861280"/>
+        <c:axId val="509856688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="509861280"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>ストライプのインデックス</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509856688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="509856688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="eaVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="ja-JP" altLang="en-US"/>
+                  <a:t>画素値差分の合計値</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="eaVert" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="ja-JP"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ja-JP"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="509861280"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ja-JP"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ja-JP"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>117475</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="グラフ 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{096F403E-233C-4EA8-B530-A5378B59A21F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -404,10 +1652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C88D624-B51F-4DAD-B676-E742C893BD41}">
-  <dimension ref="A1:M12"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -655,9 +1903,181 @@
         <v>1731</v>
       </c>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>23067</v>
+      </c>
+      <c r="E13">
+        <v>28716</v>
+      </c>
+      <c r="G13">
+        <v>22932</v>
+      </c>
+      <c r="I13">
+        <v>12297</v>
+      </c>
+      <c r="K13">
+        <v>5265</v>
+      </c>
+      <c r="M13">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14">
+        <v>35037.5</v>
+      </c>
+      <c r="E14">
+        <v>28716</v>
+      </c>
+      <c r="G14">
+        <v>29175.75</v>
+      </c>
+      <c r="I14">
+        <v>17604.5</v>
+      </c>
+      <c r="K14">
+        <v>8615.25</v>
+      </c>
+      <c r="M14">
+        <v>4770</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0019AE0-927C-44AF-A529-BC8169B1E11C}">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2">
+        <v>600</v>
+      </c>
+      <c r="B2">
+        <v>19536</v>
+      </c>
+      <c r="C2">
+        <v>25995</v>
+      </c>
+      <c r="D2">
+        <v>19293</v>
+      </c>
+      <c r="E2">
+        <v>11034</v>
+      </c>
+      <c r="F2">
+        <v>4401</v>
+      </c>
+      <c r="G2">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3">
+        <v>600</v>
+      </c>
+      <c r="B3">
+        <v>29892.5</v>
+      </c>
+      <c r="C3">
+        <v>25995</v>
+      </c>
+      <c r="D3">
+        <v>25633.5</v>
+      </c>
+      <c r="E3">
+        <v>15521.5</v>
+      </c>
+      <c r="F3">
+        <v>8320.75</v>
+      </c>
+      <c r="G3">
+        <v>4071</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>23067</v>
+      </c>
+      <c r="C4">
+        <v>28716</v>
+      </c>
+      <c r="D4">
+        <v>22932</v>
+      </c>
+      <c r="E4">
+        <v>12297</v>
+      </c>
+      <c r="F4">
+        <v>5265</v>
+      </c>
+      <c r="G4">
+        <v>4770</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5">
+        <v>30</v>
+      </c>
+      <c r="B5">
+        <v>35037.5</v>
+      </c>
+      <c r="C5">
+        <v>28716</v>
+      </c>
+      <c r="D5">
+        <v>29175.75</v>
+      </c>
+      <c r="E5">
+        <v>17604.5</v>
+      </c>
+      <c r="F5">
+        <v>8615.25</v>
+      </c>
+      <c r="G5">
+        <v>4770</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>